<commit_message>
añadir autoevaluacion de Megane
</commit_message>
<xml_diff>
--- a/1-estrategia/evaluaciones/BarretMegane-20181003.xlsx
+++ b/1-estrategia/evaluaciones/BarretMegane-20181003.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meg72\Documents\Elementos-de-la-UX\1-estrategia\evaluaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A961F6-1490-47DE-A319-F9172C1283A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A2A046-D747-4182-8BDA-01606A03C585}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="2xrU6ULNiBWh5/D1yqtqfDXEytAesw2ZR5xG+9ijSxe/fcPJZK0IGKbPDchNtQpFBAj8N/4WZgguw96FdrEMJA==" workbookSaltValue="Spg6VbYbpLv/Iy25VR1+Sw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -942,8 +942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
@@ -1238,15 +1238,15 @@
       </c>
       <c r="D20" s="33">
         <f>D21*0.33+D22*0.24+D23*0.23+D24/3*0.19</f>
-        <v>0.8</v>
+        <v>0.92666666666666675</v>
       </c>
       <c r="E20" s="33">
         <f t="shared" ref="E20:G20" si="1">E21*0.33+E22*0.24+E23*0.23+E24/3*0.19</f>
-        <v>0.57000000000000006</v>
+        <v>0.99</v>
       </c>
       <c r="F20" s="33">
         <f t="shared" si="1"/>
-        <v>0.57000000000000006</v>
+        <v>0.99</v>
       </c>
       <c r="G20" s="33">
         <f t="shared" si="1"/>
@@ -1299,8 +1299,12 @@
       <c r="D23" s="4">
         <v>1</v>
       </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
+      <c r="E23" s="4">
+        <v>1</v>
+      </c>
+      <c r="F23" s="4">
+        <v>1</v>
+      </c>
       <c r="G23" s="5"/>
       <c r="H23" s="36"/>
       <c r="J23" s="47"/>
@@ -1310,9 +1314,15 @@
       <c r="C24" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
+      <c r="D24" s="3">
+        <v>2</v>
+      </c>
+      <c r="E24" s="3">
+        <v>3</v>
+      </c>
+      <c r="F24" s="3">
+        <v>3</v>
+      </c>
       <c r="G24" s="3"/>
       <c r="H24" s="36"/>
       <c r="J24" s="30"/>
@@ -1324,15 +1334,15 @@
       </c>
       <c r="D25" s="33">
         <f>D26*0.38+D27/3*0.32+D28/3*0.17+D29*0.13</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" s="33">
         <f t="shared" ref="E25:G25" si="2">E26*0.38+E27/3*0.32+E28/3*0.17+E29*0.13</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" s="33">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" s="33">
         <f t="shared" si="2"/>
@@ -1346,9 +1356,15 @@
       <c r="C26" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
+      <c r="D26" s="5">
+        <v>1</v>
+      </c>
+      <c r="E26" s="5">
+        <v>1</v>
+      </c>
+      <c r="F26" s="5">
+        <v>1</v>
+      </c>
       <c r="G26" s="5"/>
       <c r="H26" s="36"/>
       <c r="J26" s="30"/>
@@ -1358,9 +1374,15 @@
       <c r="C27" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
+      <c r="D27" s="4">
+        <v>3</v>
+      </c>
+      <c r="E27" s="4">
+        <v>3</v>
+      </c>
+      <c r="F27" s="4">
+        <v>3</v>
+      </c>
       <c r="G27" s="4"/>
       <c r="H27" s="36"/>
       <c r="J27" s="30"/>
@@ -1370,9 +1392,15 @@
       <c r="C28" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
+      <c r="D28" s="4">
+        <v>3</v>
+      </c>
+      <c r="E28" s="4">
+        <v>3</v>
+      </c>
+      <c r="F28" s="4">
+        <v>3</v>
+      </c>
       <c r="G28" s="4"/>
       <c r="H28" s="36"/>
       <c r="J28" s="30"/>
@@ -1382,9 +1410,15 @@
       <c r="C29" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
+      <c r="D29" s="4">
+        <v>1</v>
+      </c>
+      <c r="E29" s="4">
+        <v>1</v>
+      </c>
+      <c r="F29" s="4">
+        <v>1</v>
+      </c>
       <c r="G29" s="4"/>
       <c r="H29" s="36"/>
       <c r="J29" s="30"/>

</xml_diff>